<commit_message>
added snowflake symbole to dictionnary and images. corrected xlsx template
</commit_message>
<xml_diff>
--- a/data_example/20161216_snowpit.xlsx
+++ b/data_example/20161216_snowpit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t xml:space="preserve">Snowpit form for Snowpyt package</t>
   </si>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Sample</t>
   </si>
   <si>
-    <t xml:space="preserve">Layer #, from top to bottom</t>
+    <t xml:space="preserve">Layer ID</t>
   </si>
   <si>
     <t xml:space="preserve">Top [cm]</t>
@@ -199,6 +199,9 @@
     <t xml:space="preserve">Type 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Type 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diameter min [mm]</t>
   </si>
   <si>
@@ -214,7 +217,7 @@
     <t xml:space="preserve">Depth Center [cm]</t>
   </si>
   <si>
-    <t xml:space="preserve">Snow Density [g/cm³]</t>
+    <t xml:space="preserve">Snow Density [g/cm3]</t>
   </si>
   <si>
     <t xml:space="preserve">Depth [cm]</t>
@@ -229,7 +232,7 @@
     <t xml:space="preserve">Naaa</t>
   </si>
   <si>
-    <t xml:space="preserve">refrozen melt cluster</t>
+    <t xml:space="preserve">rounded polycrystals</t>
   </si>
   <si>
     <t xml:space="preserve">nan</t>
@@ -503,33 +506,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="1.75510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,20 +838,21 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="7"/>
+      <c r="L43" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L43" s="7"/>
       <c r="M43" s="7"/>
-      <c r="N43" s="5" t="s">
+      <c r="N43" s="7"/>
+      <c r="O43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O43" s="7"/>
       <c r="P43" s="7"/>
-      <c r="Q43" s="5" t="s">
+      <c r="Q43" s="7"/>
+      <c r="R43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
     </row>
     <row r="44" s="14" customFormat="true" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
@@ -881,26 +882,29 @@
       <c r="I44" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="12" t="s">
+      <c r="J44" s="12" t="s">
         <v>63</v>
       </c>
+      <c r="K44" s="13"/>
       <c r="L44" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>65</v>
       </c>
+      <c r="N44" s="12"/>
       <c r="O44" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="12" t="s">
-        <v>63</v>
-      </c>
+      <c r="P44" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q44" s="13"/>
       <c r="R44" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="S44" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -917,33 +921,34 @@
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
-      <c r="H45" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="I45" s="16" t="str">
-        <f aca="false">IF(H45="feast",1,IF(H45="4 finger",2,IF(H45="3 finger",3,IF(H45="2 finger",4,IF(H45="1 finger",5,IF(H45="pencil",6,IF(H45="knife",7,IF(H45="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J45" s="7"/>
-      <c r="K45" s="9" t="n">
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J45" s="16" t="str">
+        <f aca="false">IF(I45="feast",1,IF(I45="4 finger",2,IF(I45="3 finger",3,IF(I45="2 finger",4,IF(I45="1 finger",5,IF(I45="pencil",6,IF(I45="knife",7,IF(I45="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K45" s="7"/>
+      <c r="L45" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L45" s="9" t="n">
+      <c r="M45" s="9" t="n">
         <f aca="false">161.4-143</f>
         <v>18.4</v>
       </c>
-      <c r="M45" s="16"/>
-      <c r="N45" s="10" t="n">
+      <c r="N45" s="16"/>
+      <c r="O45" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="O45" s="10" t="n">
+      <c r="P45" s="10" t="n">
         <v>-8</v>
       </c>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="9" t="n">
+      <c r="Q45" s="7"/>
+      <c r="R45" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="R45" s="9" t="n">
+      <c r="S45" s="9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -958,38 +963,39 @@
         <v>2</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
-      <c r="H46" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I46" s="16" t="str">
-        <f aca="false">IF(H46="feast",1,IF(H46="4 finger",2,IF(H46="3 finger",3,IF(H46="2 finger",4,IF(H46="1 finger",5,IF(H46="pencil",6,IF(H46="knife",7,IF(H46="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J46" s="7"/>
-      <c r="K46" s="10" t="n">
+      <c r="H46" s="15"/>
+      <c r="I46" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J46" s="16" t="str">
+        <f aca="false">IF(I46="feast",1,IF(I46="4 finger",2,IF(I46="3 finger",3,IF(I46="2 finger",4,IF(I46="1 finger",5,IF(I46="pencil",6,IF(I46="knife",7,IF(I46="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="L46" s="10" t="n">
+      <c r="M46" s="10" t="n">
         <f aca="false">181.1-143</f>
         <v>38.1</v>
       </c>
-      <c r="M46" s="16"/>
-      <c r="N46" s="9" t="n">
+      <c r="N46" s="16"/>
+      <c r="O46" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="O46" s="9" t="n">
+      <c r="P46" s="9" t="n">
         <v>-8.7</v>
       </c>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="10" t="n">
+      <c r="Q46" s="7"/>
+      <c r="R46" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="R46" s="10" t="n">
+      <c r="S46" s="10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1007,41 +1013,42 @@
         <v>12</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F47" s="15" t="n">
+        <v>72</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G47" s="15" t="n">
+      <c r="H47" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H47" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I47" s="16" t="str">
-        <f aca="false">IF(H47="feast",1,IF(H47="4 finger",2,IF(H47="3 finger",3,IF(H47="2 finger",4,IF(H47="1 finger",5,IF(H47="pencil",6,IF(H47="knife",7,IF(H47="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J47" s="7"/>
-      <c r="K47" s="10" t="n">
+      <c r="I47" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J47" s="16" t="str">
+        <f aca="false">IF(I47="feast",1,IF(I47="4 finger",2,IF(I47="3 finger",3,IF(I47="2 finger",4,IF(I47="1 finger",5,IF(I47="pencil",6,IF(I47="knife",7,IF(I47="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K47" s="7"/>
+      <c r="L47" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="L47" s="10" t="n">
+      <c r="M47" s="10" t="n">
         <f aca="false">181-143</f>
         <v>38</v>
       </c>
-      <c r="M47" s="16"/>
-      <c r="N47" s="10" t="n">
+      <c r="N47" s="16"/>
+      <c r="O47" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="O47" s="10" t="n">
+      <c r="P47" s="10" t="n">
         <v>-3</v>
       </c>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="9" t="n">
+      <c r="Q47" s="7"/>
+      <c r="R47" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="R47" s="9" t="n">
+      <c r="S47" s="9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1059,39 +1066,40 @@
         <v>18</v>
       </c>
       <c r="E48" s="15"/>
-      <c r="F48" s="15" t="n">
+      <c r="F48" s="15"/>
+      <c r="G48" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="15" t="n">
+      <c r="H48" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="H48" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I48" s="16" t="str">
-        <f aca="false">IF(H48="feast",1,IF(H48="4 finger",2,IF(H48="3 finger",3,IF(H48="2 finger",4,IF(H48="1 finger",5,IF(H48="pencil",6,IF(H48="knife",7,IF(H48="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J48" s="7"/>
-      <c r="K48" s="10" t="n">
+      <c r="I48" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J48" s="16" t="str">
+        <f aca="false">IF(I48="feast",1,IF(I48="4 finger",2,IF(I48="3 finger",3,IF(I48="2 finger",4,IF(I48="1 finger",5,IF(I48="pencil",6,IF(I48="knife",7,IF(I48="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K48" s="7"/>
+      <c r="L48" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="L48" s="10" t="n">
+      <c r="M48" s="10" t="n">
         <f aca="false">185.4-143</f>
         <v>42.4</v>
       </c>
-      <c r="M48" s="16"/>
-      <c r="N48" s="10" t="n">
+      <c r="N48" s="16"/>
+      <c r="O48" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="O48" s="10" t="n">
+      <c r="P48" s="10" t="n">
         <v>-2</v>
       </c>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="10" t="n">
+      <c r="Q48" s="7"/>
+      <c r="R48" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="R48" s="10" t="n">
+      <c r="S48" s="10" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1109,39 +1117,40 @@
         <v>12</v>
       </c>
       <c r="E49" s="15"/>
-      <c r="F49" s="15" t="n">
+      <c r="F49" s="15"/>
+      <c r="G49" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G49" s="15" t="n">
+      <c r="H49" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H49" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I49" s="16" t="str">
-        <f aca="false">IF(H49="feast",1,IF(H49="4 finger",2,IF(H49="3 finger",3,IF(H49="2 finger",4,IF(H49="1 finger",5,IF(H49="pencil",6,IF(H49="knife",7,IF(H49="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J49" s="7"/>
-      <c r="K49" s="10" t="n">
+      <c r="I49" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J49" s="16" t="str">
+        <f aca="false">IF(I49="feast",1,IF(I49="4 finger",2,IF(I49="3 finger",3,IF(I49="2 finger",4,IF(I49="1 finger",5,IF(I49="pencil",6,IF(I49="knife",7,IF(I49="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K49" s="7"/>
+      <c r="L49" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="L49" s="10" t="n">
+      <c r="M49" s="10" t="n">
         <f aca="false">181.8-143</f>
         <v>38.8</v>
       </c>
-      <c r="M49" s="16"/>
-      <c r="N49" s="10" t="n">
+      <c r="N49" s="16"/>
+      <c r="O49" s="10" t="n">
         <v>11.5</v>
       </c>
-      <c r="O49" s="10" t="n">
+      <c r="P49" s="10" t="n">
         <v>-1.2</v>
       </c>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="9" t="n">
+      <c r="Q49" s="7"/>
+      <c r="R49" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="R49" s="9" t="n">
+      <c r="S49" s="9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1159,33 +1168,34 @@
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
-      <c r="H50" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I50" s="16" t="str">
-        <f aca="false">IF(H50="feast",1,IF(H50="4 finger",2,IF(H50="3 finger",3,IF(H50="2 finger",4,IF(H50="1 finger",5,IF(H50="pencil",6,IF(H50="knife",7,IF(H50="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J50" s="7"/>
-      <c r="K50" s="10" t="n">
+      <c r="H50" s="15"/>
+      <c r="I50" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J50" s="16" t="str">
+        <f aca="false">IF(I50="feast",1,IF(I50="4 finger",2,IF(I50="3 finger",3,IF(I50="2 finger",4,IF(I50="1 finger",5,IF(I50="pencil",6,IF(I50="knife",7,IF(I50="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K50" s="7"/>
+      <c r="L50" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="L50" s="10" t="n">
+      <c r="M50" s="10" t="n">
         <f aca="false">181.3-143</f>
         <v>38.3</v>
       </c>
-      <c r="M50" s="16"/>
-      <c r="N50" s="10" t="n">
+      <c r="N50" s="16"/>
+      <c r="O50" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="O50" s="10" t="n">
+      <c r="P50" s="10" t="n">
         <v>-0.9</v>
       </c>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="10" t="n">
+      <c r="Q50" s="7"/>
+      <c r="R50" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="R50" s="10" t="n">
+      <c r="S50" s="10" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1205,34 +1215,35 @@
       <c r="E51" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="15" t="n">
+      <c r="F51" s="15"/>
+      <c r="G51" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G51" s="15" t="n">
+      <c r="H51" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H51" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I51" s="16" t="str">
-        <f aca="false">IF(H51="feast",1,IF(H51="4 finger",2,IF(H51="3 finger",3,IF(H51="2 finger",4,IF(H51="1 finger",5,IF(H51="pencil",6,IF(H51="knife",7,IF(H51="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J51" s="7"/>
-      <c r="K51" s="10"/>
+      <c r="I51" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J51" s="16" t="str">
+        <f aca="false">IF(I51="feast",1,IF(I51="4 finger",2,IF(I51="3 finger",3,IF(I51="2 finger",4,IF(I51="1 finger",5,IF(I51="pencil",6,IF(I51="knife",7,IF(I51="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K51" s="7"/>
       <c r="L51" s="10"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="10" t="n">
+      <c r="M51" s="10"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="O51" s="10" t="n">
+      <c r="P51" s="10" t="n">
         <v>-0.7</v>
       </c>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="9" t="n">
+      <c r="Q51" s="7"/>
+      <c r="R51" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="R51" s="9" t="n">
+      <c r="S51" s="9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1250,28 +1261,29 @@
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I52" s="16" t="str">
-        <f aca="false">IF(H52="feast",1,IF(H52="4 finger",2,IF(H52="3 finger",3,IF(H52="2 finger",4,IF(H52="1 finger",5,IF(H52="pencil",6,IF(H52="knife",7,IF(H52="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J52" s="7"/>
-      <c r="K52" s="10"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J52" s="16" t="str">
+        <f aca="false">IF(I52="feast",1,IF(I52="4 finger",2,IF(I52="3 finger",3,IF(I52="2 finger",4,IF(I52="1 finger",5,IF(I52="pencil",6,IF(I52="knife",7,IF(I52="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K52" s="7"/>
       <c r="L52" s="10"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="10" t="n">
+      <c r="M52" s="10"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="O52" s="10" t="n">
+      <c r="P52" s="10" t="n">
         <v>-0.5</v>
       </c>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="10" t="n">
+      <c r="Q52" s="7"/>
+      <c r="R52" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="R52" s="10" t="n">
+      <c r="S52" s="10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1291,32 +1303,33 @@
       <c r="E53" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="15" t="n">
+      <c r="F53" s="15"/>
+      <c r="G53" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G53" s="15" t="n">
+      <c r="H53" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H53" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I53" s="16" t="str">
-        <f aca="false">IF(H53="feast",1,IF(H53="4 finger",2,IF(H53="3 finger",3,IF(H53="2 finger",4,IF(H53="1 finger",5,IF(H53="pencil",6,IF(H53="knife",7,IF(H53="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J53" s="7"/>
-      <c r="K53" s="10"/>
+      <c r="I53" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J53" s="16" t="str">
+        <f aca="false">IF(I53="feast",1,IF(I53="4 finger",2,IF(I53="3 finger",3,IF(I53="2 finger",4,IF(I53="1 finger",5,IF(I53="pencil",6,IF(I53="knife",7,IF(I53="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K53" s="7"/>
       <c r="L53" s="10"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="10" t="n">
+      <c r="M53" s="10"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="O53" s="10" t="n">
+      <c r="P53" s="10" t="n">
         <v>-0.6</v>
       </c>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="9"/>
+      <c r="Q53" s="7"/>
       <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="n">
@@ -1332,26 +1345,27 @@
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I54" s="16" t="str">
-        <f aca="false">IF(H54="feast",1,IF(H54="4 finger",2,IF(H54="3 finger",3,IF(H54="2 finger",4,IF(H54="1 finger",5,IF(H54="pencil",6,IF(H54="knife",7,IF(H54="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J54" s="7"/>
-      <c r="K54" s="10"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J54" s="16" t="str">
+        <f aca="false">IF(I54="feast",1,IF(I54="4 finger",2,IF(I54="3 finger",3,IF(I54="2 finger",4,IF(I54="1 finger",5,IF(I54="pencil",6,IF(I54="knife",7,IF(I54="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K54" s="7"/>
       <c r="L54" s="10"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="10" t="n">
+      <c r="M54" s="10"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="O54" s="10" t="n">
+      <c r="P54" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="10"/>
+      <c r="Q54" s="7"/>
       <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="n">
@@ -1369,28 +1383,29 @@
       <c r="E55" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="15" t="n">
+      <c r="F55" s="15"/>
+      <c r="G55" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G55" s="15" t="n">
+      <c r="H55" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H55" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I55" s="16" t="str">
-        <f aca="false">IF(H55="feast",1,IF(H55="4 finger",2,IF(H55="3 finger",3,IF(H55="2 finger",4,IF(H55="1 finger",5,IF(H55="pencil",6,IF(H55="knife",7,IF(H55="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J55" s="7"/>
-      <c r="K55" s="10"/>
+      <c r="I55" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J55" s="16" t="str">
+        <f aca="false">IF(I55="feast",1,IF(I55="4 finger",2,IF(I55="3 finger",3,IF(I55="2 finger",4,IF(I55="1 finger",5,IF(I55="pencil",6,IF(I55="knife",7,IF(I55="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K55" s="7"/>
       <c r="L55" s="10"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="7"/>
       <c r="O55" s="10"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="9"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="7"/>
       <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="n">
@@ -1406,22 +1421,23 @@
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I56" s="16" t="str">
-        <f aca="false">IF(H56="feast",1,IF(H56="4 finger",2,IF(H56="3 finger",3,IF(H56="2 finger",4,IF(H56="1 finger",5,IF(H56="pencil",6,IF(H56="knife",7,IF(H56="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J56" s="7"/>
-      <c r="K56" s="10"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J56" s="16" t="str">
+        <f aca="false">IF(I56="feast",1,IF(I56="4 finger",2,IF(I56="3 finger",3,IF(I56="2 finger",4,IF(I56="1 finger",5,IF(I56="pencil",6,IF(I56="knife",7,IF(I56="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K56" s="7"/>
       <c r="L56" s="10"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="7"/>
       <c r="O56" s="10"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="7"/>
       <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="n">
@@ -1439,28 +1455,29 @@
       <c r="E57" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="15" t="n">
+      <c r="F57" s="15"/>
+      <c r="G57" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G57" s="15" t="n">
+      <c r="H57" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H57" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I57" s="16" t="str">
-        <f aca="false">IF(H57="feast",1,IF(H57="4 finger",2,IF(H57="3 finger",3,IF(H57="2 finger",4,IF(H57="1 finger",5,IF(H57="pencil",6,IF(H57="knife",7,IF(H57="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J57" s="7"/>
-      <c r="K57" s="10"/>
+      <c r="I57" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J57" s="16" t="str">
+        <f aca="false">IF(I57="feast",1,IF(I57="4 finger",2,IF(I57="3 finger",3,IF(I57="2 finger",4,IF(I57="1 finger",5,IF(I57="pencil",6,IF(I57="knife",7,IF(I57="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K57" s="7"/>
       <c r="L57" s="10"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="7"/>
       <c r="O57" s="10"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="9"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="7"/>
       <c r="R57" s="9"/>
+      <c r="S57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="n">
@@ -1476,22 +1493,23 @@
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I58" s="16" t="str">
-        <f aca="false">IF(H58="feast",1,IF(H58="4 finger",2,IF(H58="3 finger",3,IF(H58="2 finger",4,IF(H58="1 finger",5,IF(H58="pencil",6,IF(H58="knife",7,IF(H58="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="J58" s="7"/>
-      <c r="K58" s="10"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J58" s="16" t="str">
+        <f aca="false">IF(I58="feast",1,IF(I58="4 finger",2,IF(I58="3 finger",3,IF(I58="2 finger",4,IF(I58="1 finger",5,IF(I58="pencil",6,IF(I58="knife",7,IF(I58="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="K58" s="7"/>
       <c r="L58" s="10"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="7"/>
       <c r="O58" s="10"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="7"/>
       <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="n">
@@ -1509,20 +1527,21 @@
       <c r="E59" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="15" t="n">
+      <c r="F59" s="15"/>
+      <c r="G59" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G59" s="15" t="n">
+      <c r="H59" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H59" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I59" s="16" t="str">
-        <f aca="false">IF(H59="feast",1,IF(H59="4 finger",2,IF(H59="3 finger",3,IF(H59="2 finger",4,IF(H59="1 finger",5,IF(H59="pencil",6,IF(H59="knife",7,IF(H59="nan","NaN","NaN"))))))))</f>
-        <v>NaN</v>
-      </c>
-      <c r="P59" s="7"/>
+      <c r="I59" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J59" s="16" t="str">
+        <f aca="false">IF(I59="feast",1,IF(I59="4 finger",2,IF(I59="3 finger",3,IF(I59="2 finger",4,IF(I59="1 finger",5,IF(I59="pencil",6,IF(I59="knife",7,IF(I59="nan","NaN","NaN"))))))))</f>
+        <v>NaN</v>
+      </c>
+      <c r="Q59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="n">
@@ -1537,14 +1556,15 @@
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="15" t="n">
+      <c r="G60" s="15"/>
+      <c r="H60" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="H60" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I60" s="16" t="str">
-        <f aca="false">IF(H60="feast",1,IF(H60="4 finger",2,IF(H60="3 finger",3,IF(H60="2 finger",4,IF(H60="1 finger",5,IF(H60="pencil",6,IF(H60="knife",7,IF(H60="nan","NaN","NaN"))))))))</f>
+      <c r="I60" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J60" s="16" t="str">
+        <f aca="false">IF(I60="feast",1,IF(I60="4 finger",2,IF(I60="3 finger",3,IF(I60="2 finger",4,IF(I60="1 finger",5,IF(I60="pencil",6,IF(I60="knife",7,IF(I60="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1564,17 +1584,18 @@
       <c r="E61" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="15" t="n">
+      <c r="F61" s="15"/>
+      <c r="G61" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="G61" s="15" t="n">
+      <c r="H61" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="H61" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I61" s="16" t="str">
-        <f aca="false">IF(H61="feast",1,IF(H61="4 finger",2,IF(H61="3 finger",3,IF(H61="2 finger",4,IF(H61="1 finger",5,IF(H61="pencil",6,IF(H61="knife",7,IF(H61="nan","NaN","NaN"))))))))</f>
+      <c r="I61" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J61" s="16" t="str">
+        <f aca="false">IF(I61="feast",1,IF(I61="4 finger",2,IF(I61="3 finger",3,IF(I61="2 finger",4,IF(I61="1 finger",5,IF(I61="pencil",6,IF(I61="knife",7,IF(I61="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1590,17 +1611,18 @@
         <v>29</v>
       </c>
       <c r="E62" s="15"/>
-      <c r="F62" s="15" t="n">
+      <c r="F62" s="15"/>
+      <c r="G62" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="G62" s="15" t="n">
+      <c r="H62" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="H62" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I62" s="16" t="str">
-        <f aca="false">IF(H62="feast",1,IF(H62="4 finger",2,IF(H62="3 finger",3,IF(H62="2 finger",4,IF(H62="1 finger",5,IF(H62="pencil",6,IF(H62="knife",7,IF(H62="nan","NaN","NaN"))))))))</f>
+      <c r="I62" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J62" s="16" t="str">
+        <f aca="false">IF(I62="feast",1,IF(I62="4 finger",2,IF(I62="3 finger",3,IF(I62="2 finger",4,IF(I62="1 finger",5,IF(I62="pencil",6,IF(I62="knife",7,IF(I62="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1620,17 +1642,18 @@
       <c r="E63" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="15" t="n">
+      <c r="F63" s="15"/>
+      <c r="G63" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="G63" s="15" t="n">
+      <c r="H63" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="H63" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I63" s="16" t="str">
-        <f aca="false">IF(H63="feast",1,IF(H63="4 finger",2,IF(H63="3 finger",3,IF(H63="2 finger",4,IF(H63="1 finger",5,IF(H63="pencil",6,IF(H63="knife",7,IF(H63="nan","NaN","NaN"))))))))</f>
+      <c r="I63" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J63" s="16" t="str">
+        <f aca="false">IF(I63="feast",1,IF(I63="4 finger",2,IF(I63="3 finger",3,IF(I63="2 finger",4,IF(I63="1 finger",5,IF(I63="pencil",6,IF(I63="knife",7,IF(I63="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1645,20 +1668,21 @@
         <v>27</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E64" s="15"/>
-      <c r="F64" s="15" t="n">
+      <c r="F64" s="15"/>
+      <c r="G64" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G64" s="15" t="n">
+      <c r="H64" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="H64" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I64" s="16" t="str">
-        <f aca="false">IF(H64="feast",1,IF(H64="4 finger",2,IF(H64="3 finger",3,IF(H64="2 finger",4,IF(H64="1 finger",5,IF(H64="pencil",6,IF(H64="knife",7,IF(H64="nan","NaN","NaN"))))))))</f>
+      <c r="I64" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" s="16" t="str">
+        <f aca="false">IF(I64="feast",1,IF(I64="4 finger",2,IF(I64="3 finger",3,IF(I64="2 finger",4,IF(I64="1 finger",5,IF(I64="pencil",6,IF(I64="knife",7,IF(I64="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1673,20 +1697,21 @@
         <v>38</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E65" s="15"/>
-      <c r="F65" s="15" t="n">
+      <c r="F65" s="15"/>
+      <c r="G65" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G65" s="15" t="n">
+      <c r="H65" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="H65" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I65" s="16" t="str">
-        <f aca="false">IF(H65="feast",1,IF(H65="4 finger",2,IF(H65="3 finger",3,IF(H65="2 finger",4,IF(H65="1 finger",5,IF(H65="pencil",6,IF(H65="knife",7,IF(H65="nan","NaN","NaN"))))))))</f>
+      <c r="I65" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J65" s="16" t="str">
+        <f aca="false">IF(I65="feast",1,IF(I65="4 finger",2,IF(I65="3 finger",3,IF(I65="2 finger",4,IF(I65="1 finger",5,IF(I65="pencil",6,IF(I65="knife",7,IF(I65="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>
@@ -1706,11 +1731,12 @@
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
-      <c r="H66" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I66" s="16" t="str">
-        <f aca="false">IF(H66="feast",1,IF(H66="4 finger",2,IF(H66="3 finger",3,IF(H66="2 finger",4,IF(H66="1 finger",5,IF(H66="pencil",6,IF(H66="knife",7,IF(H66="nan","NaN","NaN"))))))))</f>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J66" s="16" t="str">
+        <f aca="false">IF(I66="feast",1,IF(I66="4 finger",2,IF(I66="3 finger",3,IF(I66="2 finger",4,IF(I66="1 finger",5,IF(I66="pencil",6,IF(I66="knife",7,IF(I66="nan","NaN","NaN"))))))))</f>
         <v>NaN</v>
       </c>
     </row>

</xml_diff>